<commit_message>
New feature: Payment to vendor
</commit_message>
<xml_diff>
--- a/Temp/CostAllocation.xlsx
+++ b/Temp/CostAllocation.xlsx
@@ -666,696 +666,696 @@
     </row>
   </sheetData>
   <dataValidations count="198">
-    <dataValidation type="list" sqref="A2" xr:uid="{3EFE45E7-DACC-46B7-BBCC-A20D054133A9}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B2" xr:uid="{0F171291-9AFC-42BF-A6BB-218BC8F2811C}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A3" xr:uid="{404A342E-4350-41B9-8159-C0638A186F08}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B3" xr:uid="{E6F2C32F-E84B-4729-A477-56F1716C82F3}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A4" xr:uid="{54DBA742-72DF-4176-82F9-373B0EBB5B80}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B4" xr:uid="{DDE77165-A358-46A8-801E-C714C1F19949}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A5" xr:uid="{3BD681AD-5CF6-4FA9-B052-897D93ED74AC}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B5" xr:uid="{7738C4BE-45C9-477D-B926-0FD771C25100}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A6" xr:uid="{B1D5D4D6-5C7E-4AA2-93B4-AA2675B203FC}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B6" xr:uid="{8F24F601-5FA6-49FE-A2FB-1471F35FD74F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A7" xr:uid="{D944BEDD-F2C7-4DC6-8E91-B1EC5B4FCDD2}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B7" xr:uid="{F10AC08F-7B31-498C-86FE-718364CBF1C7}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A8" xr:uid="{7798964D-5E84-4A10-BBA8-7723F98AE21A}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B8" xr:uid="{5D8B9B97-A9C8-4DEE-92AB-ABA8B0236EC2}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A9" xr:uid="{B6B01354-2078-47CA-AE98-5C1593D4744F}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B9" xr:uid="{7AA1F30F-47EB-45CE-BB92-3231B1ECB3DC}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A10" xr:uid="{C86BF98B-6348-4A01-BDAD-FEA0EC5BA5EA}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B10" xr:uid="{EA32207A-D111-4195-B23C-502EE2C19CDD}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A11" xr:uid="{87BE6876-B208-4956-A96D-4C20CFBD487A}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B11" xr:uid="{00C2EA10-B950-44BB-A839-401FB6C64EFE}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A12" xr:uid="{F1F63993-7DFC-405E-A695-CD5099349484}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B12" xr:uid="{55EDAC42-0665-4F4F-B767-FF156C5DB801}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A13" xr:uid="{EB23749C-CDB2-4869-BDC3-671193D7F884}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B13" xr:uid="{0EB0B6D2-0D2F-4C31-B4C5-F4B833F6C504}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A14" xr:uid="{96C13205-8425-4B0E-8D39-B4EB40AD8DA2}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B14" xr:uid="{50285CC8-FE3C-44C9-BF3B-564CD15A2711}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A15" xr:uid="{94648BB0-FC68-49F1-B80C-D091B8DF8515}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B15" xr:uid="{E398C469-0F27-4FF9-B0CB-1FE818092B5E}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A16" xr:uid="{77B64689-502D-4544-B487-4AA254267ECA}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B16" xr:uid="{DBA25473-525F-4076-8883-43FB9BE60A0A}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A17" xr:uid="{F3220B8F-AA37-40D6-9CA9-B2648074BD3C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B17" xr:uid="{CE8112E6-397F-4503-9A5E-57FDB624793D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A18" xr:uid="{FC4DF8D0-BC85-43F1-A1B1-E68BD6DD2060}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B18" xr:uid="{4D785825-CF49-49EC-A7CE-BC8B2E6FE4E0}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A19" xr:uid="{F7A68FDA-3770-4482-AEE8-C224F3094DF7}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B19" xr:uid="{8D2875DB-E935-4B1E-8A6B-D87B97900602}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A20" xr:uid="{A3706D5C-8EDF-4F70-86F7-F579CB7C4D1B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B20" xr:uid="{5FB732B5-F533-49A6-AAE2-D5C120DDB466}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A21" xr:uid="{489F8CB8-3DF5-44C1-A4F6-DDC53B7D2925}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B21" xr:uid="{931CFB5C-DEE0-4D57-A28C-8FF74A0AE415}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A22" xr:uid="{907F2A7A-DA78-40C4-90EF-B1683530018C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B22" xr:uid="{5B1E76DD-0446-4A73-9457-8A486B57B38D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A23" xr:uid="{55D186B6-4521-4D76-B68E-FBBDEA5C5442}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B23" xr:uid="{BECC3FA9-0B0A-406D-870B-AE58FADE7EBF}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A24" xr:uid="{376409CB-8569-43BA-ACC0-ECF6FE965804}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B24" xr:uid="{F7BCCED5-EDBE-4DB2-980E-BC5343378727}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A25" xr:uid="{3ED4669A-6563-4473-8786-AD4535AC30ED}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B25" xr:uid="{B9DDD9CB-345F-422C-B699-AD62A50D93F8}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A26" xr:uid="{8D876EA5-868F-40F0-A819-6CDA0DF42DBE}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B26" xr:uid="{C7A9B3AF-B383-47B0-88F5-919FEBBF28F9}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A27" xr:uid="{3F23C1BD-69A6-4474-A908-E90D2B5DDB51}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B27" xr:uid="{6BD17E65-189B-4AC6-A317-606B2073E13A}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A28" xr:uid="{423FC6DD-3977-4DCE-822A-53D426C29D34}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B28" xr:uid="{D7BF1DCE-9524-4198-9DE8-DBC51562714C}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A29" xr:uid="{77C9B163-6B79-4AC2-8473-58B3862A2917}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B29" xr:uid="{4020A5A3-E576-49D6-A9FE-6EFFA731DF35}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A30" xr:uid="{9F337F9E-32CC-4815-8579-C6DDE6CE8241}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B30" xr:uid="{843479D4-99FD-4EEE-8254-DB5A0A0D0178}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A31" xr:uid="{0D3DFD4B-E840-4919-ADC0-E295F6FD527F}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B31" xr:uid="{675E12F8-F780-4219-A7F8-66EBB37C4E37}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A32" xr:uid="{C272399D-EE52-41D0-ABC3-CD3C8D77E585}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B32" xr:uid="{97BEBEDC-560C-4DC0-8A95-7C337E182B68}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A33" xr:uid="{9E70DFF1-1B4F-4A86-8391-297C0F62F665}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B33" xr:uid="{362328D0-ECB0-4BC3-AAD9-A6BBC0677E6D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A34" xr:uid="{339BCD70-A4D9-4582-8D7B-3A3BDCC4402C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B34" xr:uid="{CC30AF84-DB5D-4805-A514-B877456B79B2}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A35" xr:uid="{72AE51A1-6853-457B-A52F-C843DE06AD32}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B35" xr:uid="{3334E32A-5764-4830-BE3B-EC8BC988FE97}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A36" xr:uid="{D5B5678F-0028-4854-8236-61467F038B58}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B36" xr:uid="{C02C0BAB-6F8E-42EB-968C-04D97D34E9F5}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A37" xr:uid="{9E4B2883-CE9A-47ED-8F04-2AF4A74A0D19}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B37" xr:uid="{E6A83FD3-26FE-47B4-A73F-D200A5BABA5B}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A38" xr:uid="{DC3DA926-C8C4-447B-9B50-5ED953232296}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B38" xr:uid="{27971378-0C9D-4E71-A5E9-1A97248CF2F8}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A39" xr:uid="{33333D31-0AF3-4895-BFA7-7B56120C4AE9}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B39" xr:uid="{7E059880-68C4-4660-A39C-BC41214435B0}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A40" xr:uid="{4761155F-5059-4715-A0D2-FC967A4A9226}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B40" xr:uid="{BFD4589B-4D7A-45F0-A7B7-34FDB3AA1105}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A41" xr:uid="{11648405-06A7-4841-8BD9-BB9C4F73A481}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B41" xr:uid="{A2AB25B8-B251-449E-BAC9-F70228513FA0}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A42" xr:uid="{8B0CECD5-A7BE-4C32-A649-E818DAF8DB63}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B42" xr:uid="{4BC1C256-15FF-40E9-AFE0-084DE839EDFB}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A43" xr:uid="{249B55A3-3294-45F8-B928-B7D5208493E6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B43" xr:uid="{B6F1B042-2270-4722-BA2E-3555A1D22493}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A44" xr:uid="{CD46F9FE-3DAA-4087-B3A2-F2835AAE4DC6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B44" xr:uid="{A0B12705-8B32-42BD-A8DA-0BF22C85E629}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A45" xr:uid="{ABFEA71D-4769-4FC0-99BB-05696DD697A4}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B45" xr:uid="{6C03286E-CB99-4632-BF59-1C2F5E9E8719}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A46" xr:uid="{2995BBED-0850-4694-A3E8-7D74DCB62A61}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B46" xr:uid="{D33C8B34-84BA-4BA2-9057-A2657F51471E}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A47" xr:uid="{B83F0BCD-ED70-448C-9F30-E121A24FEA17}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B47" xr:uid="{78A127D2-E54A-4635-850C-791E892B5A4F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A48" xr:uid="{21C3DABF-625A-4B24-A72D-4B747090036A}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B48" xr:uid="{F98012D7-1B01-42F7-B77F-2C59C166E191}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A49" xr:uid="{1A7D1BEB-D823-4683-8F2A-94B361E72CF8}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B49" xr:uid="{55A903A3-4799-4F72-904A-25D1A34A4C7E}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A50" xr:uid="{50FAAE12-5CBE-488F-9BFA-3380CD3ADADE}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B50" xr:uid="{443CF494-6AD5-4926-A6C5-84C4F530E784}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A51" xr:uid="{17D42B16-2708-40AA-BEA3-F96139D1262A}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B51" xr:uid="{8A73145E-8D2B-4745-B51F-6EA71836E697}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A52" xr:uid="{CEF00F54-2F9C-44B2-A412-EFAF9D80D387}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B52" xr:uid="{6EFCECDA-CD60-428F-AB5F-CC825D543C88}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A53" xr:uid="{4B377394-8AF4-4CB8-85BC-BC11EDD3E07C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B53" xr:uid="{E00743F6-51BB-4E29-BEFF-A261EAE9328F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A54" xr:uid="{06ED989B-0487-4CB8-AC7E-A024936C03A6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B54" xr:uid="{1A430C67-88A4-43DB-9A32-097446BE0ED7}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A55" xr:uid="{02A6EF3A-1C37-47E5-B4D9-EC3BEA22BE40}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B55" xr:uid="{23693BFE-60A9-45A7-A7A7-FD6BE3343CED}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A56" xr:uid="{A0D7B7FB-52D3-4059-9D10-262E65EF40A1}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B56" xr:uid="{B799542A-3412-40F5-8AB9-0469B399394B}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A57" xr:uid="{8C9360C8-E756-4D8C-A976-4157B6E974CE}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B57" xr:uid="{4759A605-7AB5-4F4C-AA8F-F2FF5EEDB65D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A58" xr:uid="{F46277B4-C80D-42D0-97B7-10382E4E8F16}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B58" xr:uid="{C3AEB2E4-4EAC-4188-AECE-A073341FD920}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A59" xr:uid="{907F9978-8BDE-46D6-BDE1-FD7DF5B48CF0}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B59" xr:uid="{F0C343C2-30B5-4EB8-AF07-614161D51635}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A60" xr:uid="{03B7AFD6-2ACA-4942-AD1F-BEDB4B1D1DE8}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B60" xr:uid="{BFDCAFEF-491D-49C5-8CC9-2B4245DABC40}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A61" xr:uid="{77CABFA1-5A47-4099-94A5-884C67B69EF7}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B61" xr:uid="{6E1532E9-8ED7-4228-B621-ABB0444C36A0}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A62" xr:uid="{582B46A9-953C-4B93-A350-4B72B02281E6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B62" xr:uid="{18351738-7663-476E-96AA-2DFA6747C1F4}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A63" xr:uid="{48A793D0-9ABC-46FD-8688-7F0235772C59}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B63" xr:uid="{BD73BCB0-F818-4506-9AF4-6B41E23E10A5}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A64" xr:uid="{984F15FA-4898-4237-826A-5653664E0D0D}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B64" xr:uid="{290C0E0C-B6FE-433B-90C1-7177E7DEE92B}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A65" xr:uid="{662289C9-3768-4811-B646-3702E6DAF7D4}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B65" xr:uid="{7617DBF0-C1C0-4500-B03C-4FA2FF21D84F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A66" xr:uid="{4661552A-E4C6-4A8B-80F9-81375EA06157}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B66" xr:uid="{D27C3207-7C35-4E65-87B0-8E64AA183CC8}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A67" xr:uid="{4C3CA75C-379F-47AE-A376-26E337034E86}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B67" xr:uid="{CFDF5179-D1B8-4950-8E3B-38664ED7FF08}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A68" xr:uid="{36D8C5E5-F8B2-49A3-9772-31A4F8C1F5C0}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B68" xr:uid="{4ED9617B-52F7-49E2-9EDF-9059140BEA84}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A69" xr:uid="{7753C5C0-779F-4B31-8AA2-1761D530528F}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B69" xr:uid="{E1897B02-C015-4DA4-B62B-8CCE657E99BB}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A70" xr:uid="{A6C7E5B7-20B4-4D14-801E-559B6E28B560}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B70" xr:uid="{0B22D813-06E1-4043-8DEE-A7703E3F44F1}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A71" xr:uid="{1E5A0C5F-F3AB-4791-ADC5-27C6575C450F}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B71" xr:uid="{7E42F769-AA39-4A7E-9A44-9E2BA65DA364}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A72" xr:uid="{DC859E97-7F13-4EAB-AAD9-328DCC7217F0}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B72" xr:uid="{E8270B69-B5EF-4484-8873-DD678F9060C6}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A73" xr:uid="{30DEC6F7-C360-4BCE-BC1E-D089C8FA91CD}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B73" xr:uid="{AE144DF6-3B31-4076-9162-FDB7DC1D8D04}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A74" xr:uid="{18980A74-2D2D-4877-8B33-9D169B15C231}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B74" xr:uid="{1DCB1D7C-5B0A-4ED2-872B-4589E283F719}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A75" xr:uid="{50F10DDB-8CAD-4167-A4A6-C4E1EB104BDB}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B75" xr:uid="{FBF7C058-E8BA-4E0E-9EEB-59516F4AD500}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A76" xr:uid="{92B60227-16FA-4E25-8B24-BEA67F3DD650}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B76" xr:uid="{C76927A4-D1DF-421A-91E9-F0C8A7659E1D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A77" xr:uid="{FF49923C-C6C9-43B8-8F0C-24F14D1499D1}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B77" xr:uid="{3783EFDE-473F-4138-88BF-683C98A04FB5}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A78" xr:uid="{C554D756-B6A5-4AD4-919E-B945B43E2FFC}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B78" xr:uid="{CC6914AC-CA42-4C58-9D78-96C23D6EC098}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A79" xr:uid="{D55D734B-39F2-42C0-B157-480F8F967CFE}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B79" xr:uid="{8404927F-FB9B-4309-9B21-EE0480A612AC}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A80" xr:uid="{D347C196-9D45-4F48-92D8-271B0F62F6B0}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B80" xr:uid="{D69FC1EF-C780-429B-8CD4-98AA27F4F9D3}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A81" xr:uid="{64DBBC12-F17F-46DF-8CCB-4F0A97B1E0CD}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B81" xr:uid="{4766C80C-1FFF-4DB4-ADAB-3AEF821936C7}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A82" xr:uid="{2F929DC7-0E60-4638-9D3D-818C71745E21}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B82" xr:uid="{7E945D8D-5183-4A61-9B2C-C829ECCB1CEB}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A83" xr:uid="{807C53BA-E86F-4562-B278-057AA3F755C5}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B83" xr:uid="{E9585565-B07B-4CB7-9702-BB7AA3A9157A}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A84" xr:uid="{749A8477-4106-43BA-9EC0-98409B0BDDD5}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B84" xr:uid="{C58DFC73-2927-4AD2-883A-812DDB64CE34}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A85" xr:uid="{77E529A5-C8B7-4FC1-8F54-CBA04A0479B8}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B85" xr:uid="{41D1E3DE-B190-4B41-84BD-87ED760140EB}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A86" xr:uid="{5539AE9D-9619-450C-842A-5C97B9809783}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B86" xr:uid="{460A9948-CD22-4DB0-B85B-8F1E79316C48}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A87" xr:uid="{2D70FB22-BC1E-4B39-B43D-277761E77EC5}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B87" xr:uid="{AC2FD742-24EE-4381-8800-578D458D7AD2}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A88" xr:uid="{DE7E8A62-483F-4731-9899-E374678B07AD}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B88" xr:uid="{AE8E1429-1B24-4763-A180-D103D603F419}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A89" xr:uid="{0656CC61-2E43-4CA9-BB6A-E2DF92DB7A76}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B89" xr:uid="{672BB8B4-8A77-48E8-9BBE-AF175B783BBB}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A90" xr:uid="{18E794D1-C057-430D-85E0-025657457EE1}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B90" xr:uid="{1336DF07-CB0F-4864-9EB9-BF9581A42043}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A91" xr:uid="{4EA6CD42-6924-4CFA-BB38-E830CA36F008}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B91" xr:uid="{A0ADE907-1CD5-4DA5-A99B-2F87130E4974}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A92" xr:uid="{2EA07F8D-07A5-4344-AC08-122EF3C9D122}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B92" xr:uid="{9F11353C-E85A-47FD-88E0-E68EACEB93E4}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A93" xr:uid="{B8073173-0E0D-480B-A6B8-608CB2472E21}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B93" xr:uid="{AD11E8D4-DD60-4AF1-BEA9-52F7CDB61D7E}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A94" xr:uid="{B1C839C2-EACB-4823-8102-843A69AC7FD5}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B94" xr:uid="{DB9E606A-D078-43C7-862C-A92620BC63AC}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A95" xr:uid="{6A0D9620-BDF8-4C1E-962B-486E531F1702}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B95" xr:uid="{0C75C113-A4A3-4E44-A9AE-ECACC7D7D7A1}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A96" xr:uid="{1439F983-971F-42BD-90FB-D3C8A08B761B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B96" xr:uid="{42EA4297-479F-420F-8C84-EAFCA2E4786D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A97" xr:uid="{52C18166-6239-481E-B8FB-7A7E1F34D3EB}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B97" xr:uid="{31D9C46B-959A-48E0-80BC-F8B60D753B62}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A98" xr:uid="{613231E5-9742-4DE6-8523-B9EB5F2A020B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B98" xr:uid="{CF6D4E1E-6A5A-4448-AFDE-4B3ED15A3865}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A99" xr:uid="{BDCC9631-F639-4427-869B-4A833D1726EB}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B99" xr:uid="{DD53E781-47C5-4CC4-8DEE-2CDF08306D78}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A100" xr:uid="{4B9C60EF-9163-4168-9E68-8C401167D8E1}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B100" xr:uid="{41989B24-B2FC-4F26-B4E9-E84ABFEC8484}">
+    <dataValidation type="list" sqref="A2" xr:uid="{2C2953A4-752F-4FF2-BBA2-55AFBA395657}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B2" xr:uid="{10EEB0F3-D791-467A-94E7-8CD665492A1A}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A3" xr:uid="{2FDF8936-78ED-46F5-B40D-BCDB2DF10A5C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B3" xr:uid="{011E4593-E9E4-4558-B12A-A802C625023F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A4" xr:uid="{B89447AB-29A6-4FF2-91DE-0E13482748DE}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B4" xr:uid="{67102AEE-F577-4C88-AE93-85A1DF892891}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A5" xr:uid="{E545B60C-1C9F-494B-8510-2B7D4299E9D8}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B5" xr:uid="{B8EA9EDB-31B6-46BE-B481-394FAB0E8ABE}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A6" xr:uid="{1004FDD6-F4A1-4555-95A7-F5193874F7AC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B6" xr:uid="{A172154D-D098-402E-8412-FEAD31EAFCB0}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A7" xr:uid="{AC4CA689-FEAF-4490-8E2E-B8E2D296049D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B7" xr:uid="{0D98AABF-BD84-4062-BCE1-4A7AA5BBF150}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A8" xr:uid="{2AE300A5-6287-4BF8-8D68-35E099D672FC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B8" xr:uid="{376FF6D4-E2EA-4A1A-B057-764FF55B445B}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A9" xr:uid="{236CA16C-F567-4592-BAAC-7E0842AEFF7F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B9" xr:uid="{7043022A-0246-4BF0-804D-2C49215EA43E}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A10" xr:uid="{95C26AA1-0B53-41AC-AC57-7ECBD1323508}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B10" xr:uid="{33D5B5C8-D5BC-4D54-BA7E-72189E231706}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A11" xr:uid="{6F3EDD6D-907C-4164-8795-189D971EAA88}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B11" xr:uid="{15948618-9CC9-4B5E-A022-7EF6ED2A61AA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A12" xr:uid="{42B31E4E-AD40-43DE-BBF1-7323E83A4E48}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B12" xr:uid="{BCB6D3D3-1CEF-4E8D-8636-49070C377110}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A13" xr:uid="{84FEDDE7-21D5-4C4D-9C46-5E29B98FBD65}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B13" xr:uid="{CDB252E5-469E-4124-B262-C5C755DC9BE8}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A14" xr:uid="{D049CC50-48E1-436F-81B0-3D06D2ABBEBA}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B14" xr:uid="{8F4E67CC-6DC8-4F4D-BB8F-FD470F7C4540}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A15" xr:uid="{E9ADF434-D1AD-457D-AC59-DD65E0B280B5}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B15" xr:uid="{DF14B138-D478-49A9-B884-771513CA33C1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A16" xr:uid="{3233A9AF-26E8-4490-AAFD-8EA42AC2CC18}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B16" xr:uid="{D1FFEB48-1728-433D-9BAA-A8D603670B1A}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A17" xr:uid="{CF9C3009-BE95-4273-98BA-9095CF3C22B9}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B17" xr:uid="{AA9D435D-FE90-41A2-AF6E-651B07310296}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A18" xr:uid="{B90B4027-2C69-46CC-9183-B94DBE6E06F7}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B18" xr:uid="{269E83E4-35D6-44D0-8F92-51F76F08F971}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A19" xr:uid="{AB7E5B4D-AC93-4C24-9F04-942BA140CC3D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B19" xr:uid="{BE91FF84-57CA-4C78-A7BB-8EDE5DEC2DBA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A20" xr:uid="{96703F57-A092-41F2-B030-C25ACAAA2CF2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B20" xr:uid="{7447DEEA-45FA-4F8F-8A79-15F45C5F7E03}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A21" xr:uid="{4B987E68-3D41-458D-BD77-BFEB8EF8EF24}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B21" xr:uid="{9378001B-B6A0-4EB9-BC83-FC82EA7CD8F1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A22" xr:uid="{7D2D7780-BF57-4C4B-A512-DF656A13F9B2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B22" xr:uid="{14767804-6AEA-4AAE-B67E-B5288C37F900}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A23" xr:uid="{5DBEC9CD-95CF-4C5D-988C-CAF4C5A2FB60}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B23" xr:uid="{1EF0BA95-478A-4F4F-B288-08F292855F08}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A24" xr:uid="{F69697AF-C688-48A1-AD89-8DFDFA80657B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B24" xr:uid="{77617B14-177B-4118-B51A-BD105311857D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A25" xr:uid="{DAD783C0-8A53-4E11-B1D0-D32EB64F4CFB}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B25" xr:uid="{61890A1E-D7AC-4D3F-85F7-A57C021D265E}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A26" xr:uid="{0D0ADA1B-9068-40AC-B488-78D7FF7DC296}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B26" xr:uid="{1B4E71D2-99D8-4855-9FCA-F492F0EAD825}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A27" xr:uid="{4C6201A2-9D4B-4D54-B8E0-36FE34F7E364}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B27" xr:uid="{D3A2EFD0-5ACC-4A2C-85F1-640624E9D5C5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A28" xr:uid="{9BF2D9F9-6559-478C-81B5-00A293ECBF03}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B28" xr:uid="{1A0C69B1-3BD4-403A-82EA-F5833FA71069}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A29" xr:uid="{0175B247-F128-4C96-9FCA-FFA6A77281F6}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B29" xr:uid="{1C818522-93B8-4924-9663-79DC436C0F60}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A30" xr:uid="{8F1B025B-945C-46B7-BD41-BE319A3107F5}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B30" xr:uid="{E6702A61-90FF-42D2-841A-3111B4B6D278}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A31" xr:uid="{F25D0322-B64C-4506-9992-31692F27F05B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B31" xr:uid="{8B646A91-4FC1-4352-8F71-1770FF84E804}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A32" xr:uid="{02F181C3-CAC5-4C4B-B1E2-F69627D547C5}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B32" xr:uid="{6DB324FD-411E-45F2-911A-430FB748D670}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A33" xr:uid="{74BC0BBB-90ED-4FB9-94CF-98F008F7E46D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B33" xr:uid="{7632F332-F90B-4056-AB17-D115F77B5CDB}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A34" xr:uid="{7ED2448E-6B1C-4A8D-A4EC-A5D79F4AC21F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B34" xr:uid="{A5FE24CD-0744-436E-B4D0-33475B0A51C3}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A35" xr:uid="{FAA7D25B-B897-415B-BB3C-D2EBBC05DE37}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B35" xr:uid="{29F3E3B7-E3E2-4D25-B905-D9678C429432}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A36" xr:uid="{79967D70-EAF5-4895-BCE7-6A10426990A7}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B36" xr:uid="{B6E2F0D1-18DD-40AF-A0EE-FCBAC9AA34A5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A37" xr:uid="{B04259DF-41BE-4FD6-A579-EACC8C77C667}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B37" xr:uid="{C2EB90C9-F68A-4EAD-A76A-E696DE6ADEFA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A38" xr:uid="{0CAC0E01-024F-49E3-94F7-050EE2AF64EE}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B38" xr:uid="{3D2FF0DD-4C77-4464-8706-C83A99D92503}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A39" xr:uid="{2EE882CB-0C5D-4C4C-B137-0F5D20BB1781}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B39" xr:uid="{E27E6DD3-27CE-4A26-BC48-F457D49CB3F8}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A40" xr:uid="{94E2DE79-43C8-4ED7-B36F-18DF4CFA8362}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B40" xr:uid="{5B7DED91-7069-4385-BEE6-F28EA3D6C535}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A41" xr:uid="{6EDFBB62-229B-4E8A-ADBF-964E94146D77}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B41" xr:uid="{D19A439B-373C-4D45-BCA4-A47B3D8DF9C8}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A42" xr:uid="{66FEA371-2852-4E5F-ACB7-B55D818F2CDD}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B42" xr:uid="{1B81592E-23D3-4832-A28C-C80F9BFB031F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A43" xr:uid="{948900B2-6667-49B0-B42D-F67622B63C59}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B43" xr:uid="{D962DB1A-4A1F-47C8-8D58-5860BD0D27A9}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A44" xr:uid="{213C3A04-AB5E-4C9A-BAB1-D0B7ACCE6D30}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B44" xr:uid="{43FBA064-7916-49CA-8AA1-BF97B35B0061}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A45" xr:uid="{23C36731-3A84-44D3-BF19-3392CD5F54EC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B45" xr:uid="{FCF20FA5-AC2A-4B0E-B846-33D3BDF81A8F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A46" xr:uid="{8606407C-F789-4800-8AE1-7B5A2E8AFEC2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B46" xr:uid="{32519CE2-FF03-4DDC-A760-0EA46FD1003D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A47" xr:uid="{C0DD3AFD-B904-4984-A3B2-506D6578D0D1}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B47" xr:uid="{754B8E28-4E08-46B7-8921-808711B29EFE}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A48" xr:uid="{9171C1F2-B756-45A8-9148-9DCA673D3B79}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B48" xr:uid="{CE10D935-7A82-4954-B962-D4D89165D416}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A49" xr:uid="{DE1941B3-4912-49F1-AA20-0AF82DE1560B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B49" xr:uid="{0DEC71D4-F2EB-4A97-8CD8-0F957DCCC097}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A50" xr:uid="{E0377F52-A5C1-4CDA-9ADC-080290DA3D8A}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B50" xr:uid="{BF3521AC-BA31-41F6-98A3-9E302685B483}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A51" xr:uid="{FCEC7356-143D-4A75-B258-5FC75D83DB43}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B51" xr:uid="{A08EF2FB-F0A8-4848-9398-297903E856B0}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A52" xr:uid="{E95D3D44-6244-46BE-ADD0-04042D7478B6}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B52" xr:uid="{A6ABA9C1-EB0A-46F4-ABEF-051F1739E57A}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A53" xr:uid="{9C2CC4A7-0517-4B6C-AB17-E95C38E6570D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B53" xr:uid="{659281EF-F518-4466-B195-81F04B330734}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A54" xr:uid="{7E18A362-0D54-4EA3-B154-D2D004B0E18C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B54" xr:uid="{39189CA4-1FCC-45F8-9B41-9FD6D0433EC9}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A55" xr:uid="{8B99EF75-0C2F-449F-9F8B-4EE8158229B9}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B55" xr:uid="{3D19B36F-E0D2-47BB-A7F1-2A1924B77728}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A56" xr:uid="{CCA249A3-E1EA-46BD-AAD0-FB607A5D12C9}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B56" xr:uid="{A2527B0A-ABEA-4F89-A881-0808CEA9A012}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A57" xr:uid="{6591159A-910A-494E-9234-E7D4FD7A16F2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B57" xr:uid="{F6EAC155-9FD2-4B3E-A61C-C808E0DF12AA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A58" xr:uid="{DF9EAFBD-EBAC-42D8-98A7-8D35B234F694}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B58" xr:uid="{55A7CD3E-6E29-4758-8003-47B1890B0778}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A59" xr:uid="{262446A6-C495-48AC-A296-94BFF003F336}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B59" xr:uid="{07975D51-A5B7-4C8E-A2EF-2867B418A051}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A60" xr:uid="{F9654E96-389E-41C1-B72D-CF279ED284BF}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B60" xr:uid="{07A9ADBE-CC4B-4F22-B8D6-D57DF0E7B2BE}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A61" xr:uid="{D3743C2F-E22E-433A-BB06-EF278B34FADC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B61" xr:uid="{6867D91E-8C53-4054-8639-04864AE04FDD}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A62" xr:uid="{DFECBDB7-0FE6-441D-A9E3-007AE43D30A6}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B62" xr:uid="{62A3FEA7-86BD-4120-8228-E007765CCCAC}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A63" xr:uid="{8B5EF8C7-4376-4F8A-BBED-EB5E45FD6240}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B63" xr:uid="{AF6E5D7F-F8C4-46C2-A8C6-8945F33E347F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A64" xr:uid="{562BEBA3-3063-4B75-AB7F-9B1D904A4046}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B64" xr:uid="{32F0C105-F4F8-41F6-8D5C-0B9D88515C32}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A65" xr:uid="{23EC6251-16B9-4933-B65E-C926C1D2F6C4}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B65" xr:uid="{7CBA6691-FE56-4E9C-8D02-993B1E41952B}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A66" xr:uid="{56FE638D-8BC5-4FD3-ADF5-29C54B1C80B0}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B66" xr:uid="{426BBA25-C094-41AE-A6C3-FD5D08AD57DD}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A67" xr:uid="{B32ECD80-F4DB-40DF-9908-349C89746A45}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B67" xr:uid="{F9F8B953-DDDE-4808-94A3-DF486B92273C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A68" xr:uid="{8B09E9D6-2E44-4F9D-B769-629EC29E717D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B68" xr:uid="{A6E74B36-F63F-41EC-98D5-2269F70E95C9}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A69" xr:uid="{BDE8FBBC-9330-42BF-AFE8-A8C79869BAEA}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B69" xr:uid="{530FD5A1-E432-4BD4-9CB1-4B80E1A95361}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A70" xr:uid="{34256A72-7EB2-4EAC-8162-939CC40AA936}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B70" xr:uid="{9365A846-8158-4CCA-B89B-1754D41F0764}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A71" xr:uid="{0A4EA009-E358-49ED-8BC5-4D065F01E496}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B71" xr:uid="{FA9E3849-79F8-4DE0-8194-E49EE5DA81ED}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A72" xr:uid="{266C09D9-804A-45FB-BD53-ECA22EDB93D1}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B72" xr:uid="{67C392CF-04A9-4DC7-89AE-75FD532303D5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A73" xr:uid="{DF67D0CE-2278-454A-A1E8-6D19E2D1A1D7}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B73" xr:uid="{E7FACEE7-074F-4907-82DC-5D30BEDC3A5C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A74" xr:uid="{8561813E-684F-4C12-ADC6-8521AB50438C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B74" xr:uid="{61F13C2F-438C-4517-98B6-D76F3683F4B1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A75" xr:uid="{27F935C3-6DBA-43B8-865A-6B345323D09D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B75" xr:uid="{F86B052A-02B2-4005-805A-8BB2CC3072C1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A76" xr:uid="{9FD1AF97-5E3F-444E-ADF0-FFBEC92137F6}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B76" xr:uid="{18362AC0-5ED9-4343-A757-AD0DEA936400}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A77" xr:uid="{EB53399C-922F-4497-95FD-74D91AE2A121}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B77" xr:uid="{3BBCA50D-84D2-4E50-8BD4-34EEC62A95E4}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A78" xr:uid="{F67AFAC7-63D6-4823-BA60-CC5F459EEEA8}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B78" xr:uid="{075D1E2D-BE7D-4098-8764-F2D4B2BC68AA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A79" xr:uid="{843E1F2D-3AD7-45C6-9AA3-E6FF752E4509}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B79" xr:uid="{8AD91C9A-3A24-40B5-A47D-EDB31518F74C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A80" xr:uid="{B3840EEA-3FA8-4595-9FE3-8BFB6A559A7B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B80" xr:uid="{C16E11CD-60AB-42F2-850B-EEC823CECBD1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A81" xr:uid="{CAB10222-6BAD-4A07-A0EC-284346B37DC4}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B81" xr:uid="{ADEFAC95-A519-4519-A422-0BAAF2768A89}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A82" xr:uid="{A62DE176-AD0B-4402-9424-E18AD5EBDF98}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B82" xr:uid="{0802AB6A-2776-4B6C-B01C-568248D95A2F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A83" xr:uid="{C24A1013-EA90-450E-A723-922BF1487622}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B83" xr:uid="{38533A30-2961-4478-B14F-5C58889C9131}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A84" xr:uid="{969EB0F3-BD07-4A50-B5B3-30E0493FF839}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B84" xr:uid="{9AF63BE0-BEED-4F3F-85E7-5AE7A9890B0D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A85" xr:uid="{1A257696-C237-47C7-8BD8-33044FDDBECD}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B85" xr:uid="{8F89F241-56A9-4B20-85AB-9617609C0CA6}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A86" xr:uid="{477A96A9-06A2-4049-92EF-355D61BFF08A}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B86" xr:uid="{1670F903-299C-42A3-8176-7D423B9FE41D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A87" xr:uid="{DA5E99D3-430C-4354-AC2F-EBCAF0B23BB6}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B87" xr:uid="{57D240C1-249E-4F76-9517-B71BD261C1C3}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A88" xr:uid="{2CE6E8D6-AD39-42A0-A6EC-A73E1EA4768E}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B88" xr:uid="{699F6F60-457B-4CDD-9FCC-306F26679342}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A89" xr:uid="{C26560D4-0FAC-46FB-ABEB-9CEE17B06DF7}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B89" xr:uid="{D580DF34-C83B-4503-A9B8-D34FBF85EE61}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A90" xr:uid="{D19F0622-A6E2-4445-91B7-57F77FCCD8FB}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B90" xr:uid="{275A621E-DA4F-4074-BB30-7679FF5F4FCD}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A91" xr:uid="{C733387F-9BDA-40A2-8586-B009F6C089CD}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B91" xr:uid="{24F8210F-A729-4065-ACF5-726EE00DED4D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A92" xr:uid="{5A6BAD5D-824C-45BB-A115-0922F4EFD089}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B92" xr:uid="{00CEE716-DC37-4282-89C9-EE87B5C49720}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A93" xr:uid="{63B45462-CE96-468E-A18C-3BAB0A936F1C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B93" xr:uid="{CC66D324-A1A9-46EA-919F-C3E46359EBD5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A94" xr:uid="{9BAC3DC7-25F7-4959-A09A-35CDA951A951}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B94" xr:uid="{CDD20F1C-3FB3-43AB-A5E0-E17DF8E5692F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A95" xr:uid="{04169FF1-3067-44DF-B3B4-DF7DE598DAC9}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B95" xr:uid="{36FBF3EF-BE6E-4CA4-96C0-BF495BBA3392}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A96" xr:uid="{85FC6A20-50B3-4627-B935-42D1012DEF67}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B96" xr:uid="{52BA4348-A9B5-4386-A216-D610F1FC14F9}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A97" xr:uid="{4758756C-0DDA-4F42-9176-77D63ED96E1C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B97" xr:uid="{ADCB34F0-4619-4467-8404-0A4587F06FBB}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A98" xr:uid="{63BF888B-79B2-4535-B02D-226CFE30E92B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B98" xr:uid="{31971987-582A-4A36-973D-A89CB274EE6E}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A99" xr:uid="{F7483D0E-108B-4F51-BCD9-67EAD5E54E7C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B99" xr:uid="{0AB84A70-209B-441E-ACBE-0B2AE9F2C2D8}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A100" xr:uid="{C4F7E206-6E6F-4CD2-B004-BE0A053FCD34}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B100" xr:uid="{6257FC97-A71B-406F-BDF5-E86269FB75FA}">
       <formula1>0</formula1>
       <formula2>999999</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Update: Processors' pages for Payment to Vendor module
</commit_message>
<xml_diff>
--- a/Temp/CostAllocation.xlsx
+++ b/Temp/CostAllocation.xlsx
@@ -666,696 +666,696 @@
     </row>
   </sheetData>
   <dataValidations count="198">
-    <dataValidation type="list" sqref="A2" xr:uid="{2C2953A4-752F-4FF2-BBA2-55AFBA395657}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B2" xr:uid="{10EEB0F3-D791-467A-94E7-8CD665492A1A}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A3" xr:uid="{2FDF8936-78ED-46F5-B40D-BCDB2DF10A5C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B3" xr:uid="{011E4593-E9E4-4558-B12A-A802C625023F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A4" xr:uid="{B89447AB-29A6-4FF2-91DE-0E13482748DE}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B4" xr:uid="{67102AEE-F577-4C88-AE93-85A1DF892891}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A5" xr:uid="{E545B60C-1C9F-494B-8510-2B7D4299E9D8}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B5" xr:uid="{B8EA9EDB-31B6-46BE-B481-394FAB0E8ABE}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A6" xr:uid="{1004FDD6-F4A1-4555-95A7-F5193874F7AC}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B6" xr:uid="{A172154D-D098-402E-8412-FEAD31EAFCB0}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A7" xr:uid="{AC4CA689-FEAF-4490-8E2E-B8E2D296049D}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B7" xr:uid="{0D98AABF-BD84-4062-BCE1-4A7AA5BBF150}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A8" xr:uid="{2AE300A5-6287-4BF8-8D68-35E099D672FC}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B8" xr:uid="{376FF6D4-E2EA-4A1A-B057-764FF55B445B}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A9" xr:uid="{236CA16C-F567-4592-BAAC-7E0842AEFF7F}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B9" xr:uid="{7043022A-0246-4BF0-804D-2C49215EA43E}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A10" xr:uid="{95C26AA1-0B53-41AC-AC57-7ECBD1323508}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B10" xr:uid="{33D5B5C8-D5BC-4D54-BA7E-72189E231706}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A11" xr:uid="{6F3EDD6D-907C-4164-8795-189D971EAA88}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B11" xr:uid="{15948618-9CC9-4B5E-A022-7EF6ED2A61AA}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A12" xr:uid="{42B31E4E-AD40-43DE-BBF1-7323E83A4E48}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B12" xr:uid="{BCB6D3D3-1CEF-4E8D-8636-49070C377110}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A13" xr:uid="{84FEDDE7-21D5-4C4D-9C46-5E29B98FBD65}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B13" xr:uid="{CDB252E5-469E-4124-B262-C5C755DC9BE8}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A14" xr:uid="{D049CC50-48E1-436F-81B0-3D06D2ABBEBA}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B14" xr:uid="{8F4E67CC-6DC8-4F4D-BB8F-FD470F7C4540}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A15" xr:uid="{E9ADF434-D1AD-457D-AC59-DD65E0B280B5}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B15" xr:uid="{DF14B138-D478-49A9-B884-771513CA33C1}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A16" xr:uid="{3233A9AF-26E8-4490-AAFD-8EA42AC2CC18}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B16" xr:uid="{D1FFEB48-1728-433D-9BAA-A8D603670B1A}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A17" xr:uid="{CF9C3009-BE95-4273-98BA-9095CF3C22B9}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B17" xr:uid="{AA9D435D-FE90-41A2-AF6E-651B07310296}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A18" xr:uid="{B90B4027-2C69-46CC-9183-B94DBE6E06F7}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B18" xr:uid="{269E83E4-35D6-44D0-8F92-51F76F08F971}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A19" xr:uid="{AB7E5B4D-AC93-4C24-9F04-942BA140CC3D}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B19" xr:uid="{BE91FF84-57CA-4C78-A7BB-8EDE5DEC2DBA}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A20" xr:uid="{96703F57-A092-41F2-B030-C25ACAAA2CF2}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B20" xr:uid="{7447DEEA-45FA-4F8F-8A79-15F45C5F7E03}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A21" xr:uid="{4B987E68-3D41-458D-BD77-BFEB8EF8EF24}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B21" xr:uid="{9378001B-B6A0-4EB9-BC83-FC82EA7CD8F1}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A22" xr:uid="{7D2D7780-BF57-4C4B-A512-DF656A13F9B2}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B22" xr:uid="{14767804-6AEA-4AAE-B67E-B5288C37F900}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A23" xr:uid="{5DBEC9CD-95CF-4C5D-988C-CAF4C5A2FB60}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B23" xr:uid="{1EF0BA95-478A-4F4F-B288-08F292855F08}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A24" xr:uid="{F69697AF-C688-48A1-AD89-8DFDFA80657B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B24" xr:uid="{77617B14-177B-4118-B51A-BD105311857D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A25" xr:uid="{DAD783C0-8A53-4E11-B1D0-D32EB64F4CFB}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B25" xr:uid="{61890A1E-D7AC-4D3F-85F7-A57C021D265E}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A26" xr:uid="{0D0ADA1B-9068-40AC-B488-78D7FF7DC296}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B26" xr:uid="{1B4E71D2-99D8-4855-9FCA-F492F0EAD825}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A27" xr:uid="{4C6201A2-9D4B-4D54-B8E0-36FE34F7E364}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B27" xr:uid="{D3A2EFD0-5ACC-4A2C-85F1-640624E9D5C5}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A28" xr:uid="{9BF2D9F9-6559-478C-81B5-00A293ECBF03}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B28" xr:uid="{1A0C69B1-3BD4-403A-82EA-F5833FA71069}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A29" xr:uid="{0175B247-F128-4C96-9FCA-FFA6A77281F6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B29" xr:uid="{1C818522-93B8-4924-9663-79DC436C0F60}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A30" xr:uid="{8F1B025B-945C-46B7-BD41-BE319A3107F5}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B30" xr:uid="{E6702A61-90FF-42D2-841A-3111B4B6D278}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A31" xr:uid="{F25D0322-B64C-4506-9992-31692F27F05B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B31" xr:uid="{8B646A91-4FC1-4352-8F71-1770FF84E804}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A32" xr:uid="{02F181C3-CAC5-4C4B-B1E2-F69627D547C5}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B32" xr:uid="{6DB324FD-411E-45F2-911A-430FB748D670}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A33" xr:uid="{74BC0BBB-90ED-4FB9-94CF-98F008F7E46D}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B33" xr:uid="{7632F332-F90B-4056-AB17-D115F77B5CDB}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A34" xr:uid="{7ED2448E-6B1C-4A8D-A4EC-A5D79F4AC21F}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B34" xr:uid="{A5FE24CD-0744-436E-B4D0-33475B0A51C3}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A35" xr:uid="{FAA7D25B-B897-415B-BB3C-D2EBBC05DE37}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B35" xr:uid="{29F3E3B7-E3E2-4D25-B905-D9678C429432}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A36" xr:uid="{79967D70-EAF5-4895-BCE7-6A10426990A7}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B36" xr:uid="{B6E2F0D1-18DD-40AF-A0EE-FCBAC9AA34A5}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A37" xr:uid="{B04259DF-41BE-4FD6-A579-EACC8C77C667}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B37" xr:uid="{C2EB90C9-F68A-4EAD-A76A-E696DE6ADEFA}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A38" xr:uid="{0CAC0E01-024F-49E3-94F7-050EE2AF64EE}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B38" xr:uid="{3D2FF0DD-4C77-4464-8706-C83A99D92503}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A39" xr:uid="{2EE882CB-0C5D-4C4C-B137-0F5D20BB1781}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B39" xr:uid="{E27E6DD3-27CE-4A26-BC48-F457D49CB3F8}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A40" xr:uid="{94E2DE79-43C8-4ED7-B36F-18DF4CFA8362}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B40" xr:uid="{5B7DED91-7069-4385-BEE6-F28EA3D6C535}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A41" xr:uid="{6EDFBB62-229B-4E8A-ADBF-964E94146D77}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B41" xr:uid="{D19A439B-373C-4D45-BCA4-A47B3D8DF9C8}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A42" xr:uid="{66FEA371-2852-4E5F-ACB7-B55D818F2CDD}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B42" xr:uid="{1B81592E-23D3-4832-A28C-C80F9BFB031F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A43" xr:uid="{948900B2-6667-49B0-B42D-F67622B63C59}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B43" xr:uid="{D962DB1A-4A1F-47C8-8D58-5860BD0D27A9}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A44" xr:uid="{213C3A04-AB5E-4C9A-BAB1-D0B7ACCE6D30}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B44" xr:uid="{43FBA064-7916-49CA-8AA1-BF97B35B0061}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A45" xr:uid="{23C36731-3A84-44D3-BF19-3392CD5F54EC}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B45" xr:uid="{FCF20FA5-AC2A-4B0E-B846-33D3BDF81A8F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A46" xr:uid="{8606407C-F789-4800-8AE1-7B5A2E8AFEC2}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B46" xr:uid="{32519CE2-FF03-4DDC-A760-0EA46FD1003D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A47" xr:uid="{C0DD3AFD-B904-4984-A3B2-506D6578D0D1}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B47" xr:uid="{754B8E28-4E08-46B7-8921-808711B29EFE}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A48" xr:uid="{9171C1F2-B756-45A8-9148-9DCA673D3B79}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B48" xr:uid="{CE10D935-7A82-4954-B962-D4D89165D416}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A49" xr:uid="{DE1941B3-4912-49F1-AA20-0AF82DE1560B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B49" xr:uid="{0DEC71D4-F2EB-4A97-8CD8-0F957DCCC097}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A50" xr:uid="{E0377F52-A5C1-4CDA-9ADC-080290DA3D8A}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B50" xr:uid="{BF3521AC-BA31-41F6-98A3-9E302685B483}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A51" xr:uid="{FCEC7356-143D-4A75-B258-5FC75D83DB43}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B51" xr:uid="{A08EF2FB-F0A8-4848-9398-297903E856B0}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A52" xr:uid="{E95D3D44-6244-46BE-ADD0-04042D7478B6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B52" xr:uid="{A6ABA9C1-EB0A-46F4-ABEF-051F1739E57A}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A53" xr:uid="{9C2CC4A7-0517-4B6C-AB17-E95C38E6570D}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B53" xr:uid="{659281EF-F518-4466-B195-81F04B330734}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A54" xr:uid="{7E18A362-0D54-4EA3-B154-D2D004B0E18C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B54" xr:uid="{39189CA4-1FCC-45F8-9B41-9FD6D0433EC9}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A55" xr:uid="{8B99EF75-0C2F-449F-9F8B-4EE8158229B9}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B55" xr:uid="{3D19B36F-E0D2-47BB-A7F1-2A1924B77728}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A56" xr:uid="{CCA249A3-E1EA-46BD-AAD0-FB607A5D12C9}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B56" xr:uid="{A2527B0A-ABEA-4F89-A881-0808CEA9A012}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A57" xr:uid="{6591159A-910A-494E-9234-E7D4FD7A16F2}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B57" xr:uid="{F6EAC155-9FD2-4B3E-A61C-C808E0DF12AA}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A58" xr:uid="{DF9EAFBD-EBAC-42D8-98A7-8D35B234F694}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B58" xr:uid="{55A7CD3E-6E29-4758-8003-47B1890B0778}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A59" xr:uid="{262446A6-C495-48AC-A296-94BFF003F336}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B59" xr:uid="{07975D51-A5B7-4C8E-A2EF-2867B418A051}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A60" xr:uid="{F9654E96-389E-41C1-B72D-CF279ED284BF}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B60" xr:uid="{07A9ADBE-CC4B-4F22-B8D6-D57DF0E7B2BE}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A61" xr:uid="{D3743C2F-E22E-433A-BB06-EF278B34FADC}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B61" xr:uid="{6867D91E-8C53-4054-8639-04864AE04FDD}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A62" xr:uid="{DFECBDB7-0FE6-441D-A9E3-007AE43D30A6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B62" xr:uid="{62A3FEA7-86BD-4120-8228-E007765CCCAC}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A63" xr:uid="{8B5EF8C7-4376-4F8A-BBED-EB5E45FD6240}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B63" xr:uid="{AF6E5D7F-F8C4-46C2-A8C6-8945F33E347F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A64" xr:uid="{562BEBA3-3063-4B75-AB7F-9B1D904A4046}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B64" xr:uid="{32F0C105-F4F8-41F6-8D5C-0B9D88515C32}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A65" xr:uid="{23EC6251-16B9-4933-B65E-C926C1D2F6C4}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B65" xr:uid="{7CBA6691-FE56-4E9C-8D02-993B1E41952B}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A66" xr:uid="{56FE638D-8BC5-4FD3-ADF5-29C54B1C80B0}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B66" xr:uid="{426BBA25-C094-41AE-A6C3-FD5D08AD57DD}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A67" xr:uid="{B32ECD80-F4DB-40DF-9908-349C89746A45}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B67" xr:uid="{F9F8B953-DDDE-4808-94A3-DF486B92273C}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A68" xr:uid="{8B09E9D6-2E44-4F9D-B769-629EC29E717D}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B68" xr:uid="{A6E74B36-F63F-41EC-98D5-2269F70E95C9}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A69" xr:uid="{BDE8FBBC-9330-42BF-AFE8-A8C79869BAEA}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B69" xr:uid="{530FD5A1-E432-4BD4-9CB1-4B80E1A95361}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A70" xr:uid="{34256A72-7EB2-4EAC-8162-939CC40AA936}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B70" xr:uid="{9365A846-8158-4CCA-B89B-1754D41F0764}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A71" xr:uid="{0A4EA009-E358-49ED-8BC5-4D065F01E496}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B71" xr:uid="{FA9E3849-79F8-4DE0-8194-E49EE5DA81ED}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A72" xr:uid="{266C09D9-804A-45FB-BD53-ECA22EDB93D1}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B72" xr:uid="{67C392CF-04A9-4DC7-89AE-75FD532303D5}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A73" xr:uid="{DF67D0CE-2278-454A-A1E8-6D19E2D1A1D7}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B73" xr:uid="{E7FACEE7-074F-4907-82DC-5D30BEDC3A5C}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A74" xr:uid="{8561813E-684F-4C12-ADC6-8521AB50438C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B74" xr:uid="{61F13C2F-438C-4517-98B6-D76F3683F4B1}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A75" xr:uid="{27F935C3-6DBA-43B8-865A-6B345323D09D}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B75" xr:uid="{F86B052A-02B2-4005-805A-8BB2CC3072C1}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A76" xr:uid="{9FD1AF97-5E3F-444E-ADF0-FFBEC92137F6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B76" xr:uid="{18362AC0-5ED9-4343-A757-AD0DEA936400}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A77" xr:uid="{EB53399C-922F-4497-95FD-74D91AE2A121}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B77" xr:uid="{3BBCA50D-84D2-4E50-8BD4-34EEC62A95E4}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A78" xr:uid="{F67AFAC7-63D6-4823-BA60-CC5F459EEEA8}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B78" xr:uid="{075D1E2D-BE7D-4098-8764-F2D4B2BC68AA}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A79" xr:uid="{843E1F2D-3AD7-45C6-9AA3-E6FF752E4509}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B79" xr:uid="{8AD91C9A-3A24-40B5-A47D-EDB31518F74C}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A80" xr:uid="{B3840EEA-3FA8-4595-9FE3-8BFB6A559A7B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B80" xr:uid="{C16E11CD-60AB-42F2-850B-EEC823CECBD1}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A81" xr:uid="{CAB10222-6BAD-4A07-A0EC-284346B37DC4}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B81" xr:uid="{ADEFAC95-A519-4519-A422-0BAAF2768A89}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A82" xr:uid="{A62DE176-AD0B-4402-9424-E18AD5EBDF98}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B82" xr:uid="{0802AB6A-2776-4B6C-B01C-568248D95A2F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A83" xr:uid="{C24A1013-EA90-450E-A723-922BF1487622}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B83" xr:uid="{38533A30-2961-4478-B14F-5C58889C9131}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A84" xr:uid="{969EB0F3-BD07-4A50-B5B3-30E0493FF839}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B84" xr:uid="{9AF63BE0-BEED-4F3F-85E7-5AE7A9890B0D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A85" xr:uid="{1A257696-C237-47C7-8BD8-33044FDDBECD}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B85" xr:uid="{8F89F241-56A9-4B20-85AB-9617609C0CA6}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A86" xr:uid="{477A96A9-06A2-4049-92EF-355D61BFF08A}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B86" xr:uid="{1670F903-299C-42A3-8176-7D423B9FE41D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A87" xr:uid="{DA5E99D3-430C-4354-AC2F-EBCAF0B23BB6}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B87" xr:uid="{57D240C1-249E-4F76-9517-B71BD261C1C3}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A88" xr:uid="{2CE6E8D6-AD39-42A0-A6EC-A73E1EA4768E}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B88" xr:uid="{699F6F60-457B-4CDD-9FCC-306F26679342}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A89" xr:uid="{C26560D4-0FAC-46FB-ABEB-9CEE17B06DF7}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B89" xr:uid="{D580DF34-C83B-4503-A9B8-D34FBF85EE61}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A90" xr:uid="{D19F0622-A6E2-4445-91B7-57F77FCCD8FB}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B90" xr:uid="{275A621E-DA4F-4074-BB30-7679FF5F4FCD}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A91" xr:uid="{C733387F-9BDA-40A2-8586-B009F6C089CD}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B91" xr:uid="{24F8210F-A729-4065-ACF5-726EE00DED4D}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A92" xr:uid="{5A6BAD5D-824C-45BB-A115-0922F4EFD089}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B92" xr:uid="{00CEE716-DC37-4282-89C9-EE87B5C49720}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A93" xr:uid="{63B45462-CE96-468E-A18C-3BAB0A936F1C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B93" xr:uid="{CC66D324-A1A9-46EA-919F-C3E46359EBD5}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A94" xr:uid="{9BAC3DC7-25F7-4959-A09A-35CDA951A951}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B94" xr:uid="{CDD20F1C-3FB3-43AB-A5E0-E17DF8E5692F}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A95" xr:uid="{04169FF1-3067-44DF-B3B4-DF7DE598DAC9}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B95" xr:uid="{36FBF3EF-BE6E-4CA4-96C0-BF495BBA3392}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A96" xr:uid="{85FC6A20-50B3-4627-B935-42D1012DEF67}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B96" xr:uid="{52BA4348-A9B5-4386-A216-D610F1FC14F9}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A97" xr:uid="{4758756C-0DDA-4F42-9176-77D63ED96E1C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B97" xr:uid="{ADCB34F0-4619-4467-8404-0A4587F06FBB}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A98" xr:uid="{63BF888B-79B2-4535-B02D-226CFE30E92B}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B98" xr:uid="{31971987-582A-4A36-973D-A89CB274EE6E}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A99" xr:uid="{F7483D0E-108B-4F51-BCD9-67EAD5E54E7C}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B99" xr:uid="{0AB84A70-209B-441E-ACBE-0B2AE9F2C2D8}">
-      <formula1>0</formula1>
-      <formula2>999999</formula2>
-    </dataValidation>
-    <dataValidation type="list" sqref="A100" xr:uid="{C4F7E206-6E6F-4CD2-B004-BE0A053FCD34}">
-      <formula1>CostCenterList</formula1>
-    </dataValidation>
-    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B100" xr:uid="{6257FC97-A71B-406F-BDF5-E86269FB75FA}">
+    <dataValidation type="list" sqref="A2" xr:uid="{1D343961-6536-4715-B8ED-158EFBCD1E78}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B2" xr:uid="{75AFA5E1-5C9C-46CB-9BF1-EDC7852BADF5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A3" xr:uid="{33047351-FD40-42C7-8530-5C0D2358EF82}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B3" xr:uid="{332D1C23-7B5B-49DF-9F39-02375FB3E08B}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A4" xr:uid="{74A22C34-B1E8-4171-A4E9-BDEB28760A3D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B4" xr:uid="{534B0EAC-788D-4739-A42B-05BCA50B7901}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A5" xr:uid="{615613E5-A6B3-469A-9034-5F2B372F5237}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B5" xr:uid="{E24E54F5-2E01-4D39-AF01-AFA31805A7C3}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A6" xr:uid="{9E22101E-2181-459D-9854-585F2C231FBE}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B6" xr:uid="{74E7B050-88DE-4A3F-9D68-87991687DED3}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A7" xr:uid="{00BE39B5-61A9-4F28-AB18-87E1C031BE89}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B7" xr:uid="{DA860EE8-4364-4E1C-BEDE-E610593735B4}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A8" xr:uid="{2E955A54-E280-4B36-8C24-A2999A9F4B65}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B8" xr:uid="{90281998-7803-4161-A7FF-BEA7561C6E61}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A9" xr:uid="{F6BC511B-22BC-45E9-A7AA-3F6A3D9F05FA}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B9" xr:uid="{2F4449E9-30ED-4374-B977-DC9F8FA0676D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A10" xr:uid="{6E83EBF6-C0AE-4D79-BC2B-CF0C12E3AB86}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B10" xr:uid="{3AAEFA53-1FD4-4610-B829-CE891DB6505C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A11" xr:uid="{FCC23A9D-2850-4D65-9CC0-7C032AB1F4BF}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B11" xr:uid="{37E9C1E7-C17C-474C-8C0D-46340F8D8FC6}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A12" xr:uid="{9AC1F83E-2394-49B7-B148-689B6B9F3371}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B12" xr:uid="{CBAA63A1-763E-462D-BB38-B2797B22C9FD}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A13" xr:uid="{24ED5C04-57F6-428F-ABC0-0119A33DD3DC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B13" xr:uid="{FF6158E7-86AB-4779-ABAC-BE6253528A35}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A14" xr:uid="{EBD730D8-3B02-4591-A697-D44E78274AA2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B14" xr:uid="{F35D424D-459C-466C-B937-F9B1210CD0B6}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A15" xr:uid="{B732205C-7DE9-4B05-BE1C-77BA0243FF75}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B15" xr:uid="{3C300B10-70D5-4F31-9407-D017778ABE0A}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A16" xr:uid="{5A9A2138-571B-489F-9383-1E36202DFC1F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B16" xr:uid="{46087723-F179-40A1-93EA-3F5F42758119}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A17" xr:uid="{0CE2ACC5-47C9-4038-A450-40F829990CE4}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B17" xr:uid="{E08DB6DD-C208-477A-859C-83DC5C037179}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A18" xr:uid="{87AA6376-71B0-41E6-93AC-F06C5576E0FF}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B18" xr:uid="{3FFD46B0-9803-453A-9E47-6CB0E9C7DB76}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A19" xr:uid="{283D8769-5E2A-4C60-A388-FE50CD77D632}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B19" xr:uid="{144F66A0-FE96-4EB2-A725-DF54F2A88BE6}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A20" xr:uid="{2E54339D-D0A1-463A-B993-3F8794EB93EA}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B20" xr:uid="{B98BB700-6BB9-44DB-8F6D-F88B24BC4866}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A21" xr:uid="{875750CD-D960-4526-98B2-478048AB665A}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B21" xr:uid="{2364BB66-6B0C-4BA8-991C-938FDC9089EC}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A22" xr:uid="{E3CE15F6-30F0-4B15-95B6-87EC3FF6A2A2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B22" xr:uid="{6F79518C-C8CF-4946-933E-BEA982CD4230}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A23" xr:uid="{CD53A02D-D305-4533-BD0D-D11D4074DC03}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B23" xr:uid="{F1E9DCA0-4BB7-47F5-9D99-3957D1688B88}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A24" xr:uid="{C309C31F-F571-4C25-9536-E373C0765187}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B24" xr:uid="{6ACD4AFB-02CE-4D82-ABE9-EF2854B88560}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A25" xr:uid="{30B300D6-042D-45B8-BE23-5B3B44673484}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B25" xr:uid="{0555BA79-5710-48EE-B87D-E925FFD83368}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A26" xr:uid="{18D07CE0-8DAF-40AE-9B77-85F2A188622B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B26" xr:uid="{E137EFBB-DFB3-4440-97D0-F6E8E03FC227}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A27" xr:uid="{0CC8944E-6C35-4616-A3F6-B157474FD82D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B27" xr:uid="{BC5014AE-9895-413A-939A-903439D23125}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A28" xr:uid="{642C3974-9BC2-4790-AF09-65CE3AC78DEF}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B28" xr:uid="{C41FA395-22EE-428D-9089-2F5430CDE730}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A29" xr:uid="{C2DAAAB1-0A63-421E-B224-0006CA834E60}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B29" xr:uid="{23D548F8-63E4-4F1D-8BC5-94B36A2BBC5D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A30" xr:uid="{11066406-8E9E-4DC8-A33B-26F39A4E545C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B30" xr:uid="{A0C0768F-8481-4411-9157-BE76165DED58}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A31" xr:uid="{B9451D3D-9C44-49DD-AEB9-246BCE369508}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B31" xr:uid="{E545F836-0731-4A74-8634-5E759EA50D87}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A32" xr:uid="{82F0F237-C515-4B10-A658-B34C22E7618D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B32" xr:uid="{BFE9B3B9-A71D-4A6D-A973-40997C9590F3}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A33" xr:uid="{3ED6B363-A92A-4DF1-92D7-6C7BE7F7A0D7}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B33" xr:uid="{6760EB71-0E51-40C4-99EB-C44B1F828CBA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A34" xr:uid="{50B0A85A-ADD2-471E-BEC4-66CD85F6D2E8}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B34" xr:uid="{96AB2FF5-A22A-4601-AC8C-936FE75200A4}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A35" xr:uid="{017C6C6C-1E01-4CE0-AF06-29C439291745}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B35" xr:uid="{671900F4-C70B-4D98-A0C6-80080C3CFDE8}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A36" xr:uid="{1373FEC4-3775-4A5F-A33C-4D56C6EF5E07}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B36" xr:uid="{5FA319F1-2B5F-4FD2-B591-9100606B2D69}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A37" xr:uid="{61B58DB7-DA7F-4EA0-8246-A3AC5FA48174}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B37" xr:uid="{ACF0B982-D03B-47CB-9BE3-A66EEA583FDE}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A38" xr:uid="{ABB0C04E-8BAD-418B-B0E3-9AE33C0F4B80}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B38" xr:uid="{FD9B0B27-434E-4967-93E5-BDC23BB30D94}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A39" xr:uid="{FE9500E3-08D7-4D1E-BACD-6596A5D831D1}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B39" xr:uid="{BE4D5480-46E1-4622-9C84-CBB03BFF3668}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A40" xr:uid="{6DE62B52-8D27-4490-9D1C-7C4A3CE047DA}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B40" xr:uid="{FE747803-2A06-46C1-9304-054F689BC8E5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A41" xr:uid="{DF458724-D275-49A3-991B-6AF678252D43}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B41" xr:uid="{DB477294-AFC5-4C26-8318-F6E4B2E48BCA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A42" xr:uid="{7D930118-CC74-4204-8FFA-AF4123A59CB4}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B42" xr:uid="{E5FA8AC0-DA9C-4C08-B799-81043AB84F7E}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A43" xr:uid="{BC36B280-9C53-42C7-B633-30BC50CFFF17}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B43" xr:uid="{DF2C6A00-6F33-4B19-AF24-BE27EEAB6B45}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A44" xr:uid="{F2B986A1-E34F-4BCF-B609-E1A193101648}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B44" xr:uid="{A3351A4D-0E80-4766-B0A3-A068A1A660C1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A45" xr:uid="{85B8E9BC-20D2-4DED-BA07-BD698BB86154}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B45" xr:uid="{8D26FF1A-AD3D-4714-9D0B-4E5D5A90AF82}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A46" xr:uid="{13059B1A-0A95-4E50-AD27-AC324A81C3C2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B46" xr:uid="{F814B8B4-866D-45A5-96FC-905BEBFF9BAC}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A47" xr:uid="{2B28BE01-F6CE-4CD2-AB83-182E3CE70E38}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B47" xr:uid="{F1FF0F66-2128-4D7F-9384-2EE96FA41E13}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A48" xr:uid="{81DB037B-0F17-407F-B1A9-389F633DAB6F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B48" xr:uid="{E030419E-C9E8-49F4-B719-EB62457FB5DC}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A49" xr:uid="{64425482-DACC-46BB-9E20-C7B18462378C}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B49" xr:uid="{06A39D22-7230-46A4-8DDC-DABF675EF68A}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A50" xr:uid="{6206D14D-FF4B-423F-A15F-0238106A5657}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B50" xr:uid="{295156E3-23B7-4E04-9E6C-F7E13E60D4CD}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A51" xr:uid="{81B4E074-0026-4BD8-A3D1-68A17331B19B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B51" xr:uid="{6D3A673B-B4CF-47C5-A497-CEDBF85DDFA9}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A52" xr:uid="{FD90261B-B05D-4374-82DD-021ECE7DCE8D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B52" xr:uid="{A82AC6F2-79F7-4F35-82C5-F98F7CF44D87}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A53" xr:uid="{58D46023-0CA0-40B3-8710-F3D7C1DF0DA7}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B53" xr:uid="{4CFF0EB7-4D82-4B7D-B03A-EE002D621BD1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A54" xr:uid="{5C1A2AB2-1A88-42F1-B279-C0551E2A185D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B54" xr:uid="{8861F4C6-49CA-4036-81D4-7391FAA66C85}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A55" xr:uid="{03A9C593-D3C8-4964-95FB-8B99D6BA8F8F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B55" xr:uid="{F50B0F0D-A5E6-4D11-9267-5672D84D92B6}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A56" xr:uid="{84D73A2F-E043-4D74-95D6-5FBB12996C25}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B56" xr:uid="{4D8C43AE-3EF6-40AD-8F87-EFA841BB39EB}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A57" xr:uid="{555642AE-1848-49A8-89AE-4F0070B819EA}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B57" xr:uid="{37D8D61E-F0CC-45F5-B60D-8BDFFD69551D}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A58" xr:uid="{49C54163-8D0E-4CBB-B679-9247D30AA90F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B58" xr:uid="{3B5B6DDE-776A-4318-BD5E-8880A947A292}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A59" xr:uid="{A60FFB81-6A54-4ABF-9DED-73798B0E1BFF}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B59" xr:uid="{C0B86A94-C44D-4361-888E-9324A1C63E5B}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A60" xr:uid="{0A630376-3906-4881-ABD8-8BC7AC1470CE}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B60" xr:uid="{0626A3F6-0F29-427B-9E42-1566A20A9C72}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A61" xr:uid="{469993B3-39CD-4FC6-909A-43077E7B3772}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B61" xr:uid="{F87C8009-32F2-42F1-920C-9552A59525C6}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A62" xr:uid="{0E5868B8-EB3B-443F-9303-F1346CCE49F0}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B62" xr:uid="{38CAD6D5-FF87-42A3-B1DB-C2E6F7B0C116}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A63" xr:uid="{E3BA6327-1D82-4E24-87C9-9BC660038480}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B63" xr:uid="{F05478ED-D546-4DB2-AE3B-86813A5E6C59}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A64" xr:uid="{973CC7A0-6829-42E1-A5A4-9AFD06F97778}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B64" xr:uid="{58A746D5-036F-418A-99FD-CF07B45E9728}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A65" xr:uid="{7D28F62D-11A1-47E9-8C65-9B7EA2E4E8F5}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B65" xr:uid="{ADA62949-6300-487A-B9C3-94448492A264}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A66" xr:uid="{0E69F238-4E76-43E4-8697-62D1209997ED}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B66" xr:uid="{4B3D9BBD-DF2C-4F96-ACB2-C8855AB1A831}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A67" xr:uid="{B84C8391-B669-4890-AE2F-DE6ECB43EE43}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B67" xr:uid="{2C6E0ED4-A266-468B-97C8-05EED9F4D9F5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A68" xr:uid="{707EC0C9-FCBB-4812-8465-D8B9CD20EAF5}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B68" xr:uid="{A3F1138B-5D10-4DB1-A156-A0478398ACD2}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A69" xr:uid="{D1180FF2-3771-4C56-B051-C48B1EE6E802}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B69" xr:uid="{7B4510F0-9A07-4AD0-A11D-302C94A85BD1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A70" xr:uid="{E4F8D9C4-AB08-4B5C-87CA-F97B3C248D78}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B70" xr:uid="{9B5E430A-10B5-41F9-A9D2-BF8FC92BE196}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A71" xr:uid="{D136A7E1-5750-49D0-88B5-53984312ECF9}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B71" xr:uid="{AA873EEA-8E05-46DD-B791-497DB8205406}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A72" xr:uid="{32C74B4B-FE9D-4356-BB65-B4375DE1C6C2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B72" xr:uid="{CF3D61D1-0431-4BDA-A8A5-667106A9A65C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A73" xr:uid="{FDFE5136-82B2-4A9C-9C62-FF93D548B208}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B73" xr:uid="{AC417833-0B59-4D28-B4D3-68A6BF3112E9}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A74" xr:uid="{2DCA1FFE-B333-45FB-A82B-45990EFA886D}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B74" xr:uid="{B9AC2787-91EA-49AE-93BC-E1D1877A3D8C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A75" xr:uid="{28A24AB8-E1A6-43CC-9210-00AD032B33A9}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B75" xr:uid="{E9FFFB6D-A1E7-463D-BA30-0E88CECFE542}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A76" xr:uid="{07CC9BF4-8CB7-4BFB-A57B-585CA7B75EC4}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B76" xr:uid="{CD54674F-FCB4-4B07-99F1-305C03E33D63}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A77" xr:uid="{F9A6192B-81CB-42EA-B241-0C9690F03730}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B77" xr:uid="{CC5DB14D-5790-4642-9EFD-50648FB4327C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A78" xr:uid="{567255C1-FBF8-41C4-AF9A-9F30C1D40EC7}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B78" xr:uid="{8CC2E726-2427-4220-B0E8-528E23727BDE}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A79" xr:uid="{1AE32873-F5AE-4269-9CC0-FDC0543319CA}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B79" xr:uid="{F6863B04-DF98-4383-9AAC-01B56A151288}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A80" xr:uid="{D71A4226-456D-4E92-BD66-E62A90415368}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B80" xr:uid="{55D0D7EF-C5D6-4B98-A862-7D48105C2728}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A81" xr:uid="{46DFF0D1-0207-4A87-B33D-0B98725B3589}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B81" xr:uid="{16B8188D-1840-49E6-B031-695F84B4680E}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A82" xr:uid="{E65B9670-592C-4FF0-8881-141BF4683446}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B82" xr:uid="{6006B360-1BC2-47DD-8752-540BE5DB40D1}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A83" xr:uid="{623EF30E-2FEB-464A-85AC-DF890CC3A5A1}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B83" xr:uid="{D43A471B-E303-4E98-8664-112CE0862BCA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A84" xr:uid="{562662F9-480A-4054-A494-44F5AAA7973F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B84" xr:uid="{ACF00976-D6DD-4307-8500-5AA2C26BB23B}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A85" xr:uid="{3C6E9F73-08FC-4C56-9784-0BD464E22A5B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B85" xr:uid="{F675A3ED-41F4-43D9-B908-AA49CDC44EF6}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A86" xr:uid="{F5148E95-E533-4C12-B5F8-DF1F25F0B0B2}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B86" xr:uid="{D57267E0-E397-44F4-BBDB-879BEDD2738F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A87" xr:uid="{429EC393-37E9-4242-918F-E51A16DAB08A}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B87" xr:uid="{73592162-1201-4274-AB37-2F2F585213E5}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A88" xr:uid="{E1E2250F-505C-4457-AA87-623BDB5D9CEC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B88" xr:uid="{AC336E8D-8047-4EFF-8490-6273C9E69163}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A89" xr:uid="{E46CE934-2547-498C-BB9B-F6E4BD4DF3F1}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B89" xr:uid="{E957E106-0D6A-4491-9606-18809B796C66}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A90" xr:uid="{E00BBFAC-9E61-43DE-ABB9-5F721600DF49}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B90" xr:uid="{B4533ACB-4DC1-4989-91A7-66F04E743D2F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A91" xr:uid="{8341C1FC-D62B-4B47-8CE4-CE8B4D3B67B4}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B91" xr:uid="{FD5E6626-4196-44ED-B154-586496E062AA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A92" xr:uid="{1A71DDEE-4ACA-45A7-A116-DB2EDEBDF4EC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B92" xr:uid="{DA5C7BA8-AE0C-4052-B247-E57FC4FF1602}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A93" xr:uid="{9A7986AE-649D-4CD2-917C-4CEDF0E7798B}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B93" xr:uid="{564F067C-99CA-4B5C-AD2A-97ADAD0910C3}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A94" xr:uid="{71273678-026C-4445-A5D3-11E64B3F9BE6}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B94" xr:uid="{0B9FB502-23EB-4430-9F00-66E6041803DA}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A95" xr:uid="{7FCA6B76-6B3F-49D6-B9CF-2F12B2CEC1E0}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B95" xr:uid="{B436D716-81FD-403E-B9FB-50AE27EF824B}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A96" xr:uid="{DDF2DDC5-EE96-4DD3-8983-4EA68880CD77}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B96" xr:uid="{53109197-2990-4E6C-9F71-DB87AE0F305E}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A97" xr:uid="{34171F3D-4F54-46AE-8F37-80F5B74BA4FC}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B97" xr:uid="{78B705B6-22C4-466B-9435-F4B319EA730F}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A98" xr:uid="{7B1C80E6-9C12-4D30-AD56-09F0428CFFC3}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B98" xr:uid="{D2F1F499-8197-44FF-BCFD-D19C4957785C}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A99" xr:uid="{070E0933-F07B-48D4-B84E-3A8869E72EEF}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B99" xr:uid="{5AB9653A-326E-42B9-92C2-CA99DC7420F0}">
+      <formula1>0</formula1>
+      <formula2>999999</formula2>
+    </dataValidation>
+    <dataValidation type="list" sqref="A100" xr:uid="{FD756A3C-7BF8-4AF5-95D8-3559F04AE87F}">
+      <formula1>CostCenterList</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" showErrorMessage="1" errorTitle="Invalid Input" error="Please enter a valid number (decimal or integer)." sqref="B100" xr:uid="{7B9E7AD8-F07A-45C7-904D-C6172D51EAC6}">
       <formula1>0</formula1>
       <formula2>999999</formula2>
     </dataValidation>

</xml_diff>